<commit_message>
Map ready, excel writer added
</commit_message>
<xml_diff>
--- a/pdfs/emplo.xlsx
+++ b/pdfs/emplo.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,12 +11,15 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+  <si>
+    <t>test</t>
+  </si>
   <si>
     <t>Sonya</t>
   </si>
@@ -80,7 +83,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -88,9 +91,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -128,7 +131,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -198,7 +201,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -383,16 +386,16 @@
         <v>7.0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
@@ -400,16 +403,16 @@
         <v>8.0</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -417,16 +420,16 @@
         <v>9.0</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>